<commit_message>
Added fix to nan values
</commit_message>
<xml_diff>
--- a/data/raw/Recipes.xlsx
+++ b/data/raw/Recipes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="101">
   <si>
     <t>Nombre</t>
   </si>
@@ -19,6 +19,9 @@
     <t>Tipo</t>
   </si>
   <si>
+    <t>Tag</t>
+  </si>
+  <si>
     <t>Link</t>
   </si>
   <si>
@@ -124,7 +127,10 @@
     <t>https://www.bbcgoodfood.com/recipes/smoked-salmon-spaghetti-chilli-lemon</t>
   </si>
   <si>
-    <t>Macaroni and Cheese with Jalapeños and Prosciutto</t>
+    <t>Jalapeno and Chorizo Macaroni and Cheese</t>
+  </si>
+  <si>
+    <t>https://ericasrecipes.com/jalapeno-and-chorizo-macaroni-and-cheese/</t>
   </si>
   <si>
     <t>Shrimp and Zucchini Scampi</t>
@@ -229,6 +235,9 @@
     <t xml:space="preserve">Cannelloni ricotta e spinaci </t>
   </si>
   <si>
+    <t xml:space="preserve">Pasta </t>
+  </si>
+  <si>
     <t>https://www.bbcgoodfood.com/recipes/spinach-ricotta-cannelloni</t>
   </si>
   <si>
@@ -296,6 +305,15 @@
   </si>
   <si>
     <t>https://simple-veganista.com/moroccan-pumpkin-chickpea-stew/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conchiglioni ripieni </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polpettone bacon </t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/reel/ChlyURqDGey/?igshid=YmMyMTA2M2Y=</t>
   </si>
 </sst>
 </file>
@@ -579,531 +597,607 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
         <v>28</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>44</v>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>53</v>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>61</v>
+        <v>13</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>65</v>
+        <v>13</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>68</v>
+        <v>13</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>74</v>
+        <v>13</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>80</v>
+        <v>5</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>84</v>
+        <v>43</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>86</v>
+        <v>28</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>88</v>
+        <v>43</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>90</v>
+        <v>5</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>92</v>
+        <v>43</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>94</v>
+        <v>5</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="C3"/>
-    <hyperlink r:id="rId3" ref="C4"/>
-    <hyperlink r:id="rId4" ref="C5"/>
-    <hyperlink r:id="rId5" ref="C6"/>
-    <hyperlink r:id="rId6" ref="C7"/>
-    <hyperlink r:id="rId7" ref="C8"/>
-    <hyperlink r:id="rId8" ref="C9"/>
-    <hyperlink r:id="rId9" ref="C10"/>
-    <hyperlink r:id="rId10" ref="C11"/>
-    <hyperlink r:id="rId11" ref="C12"/>
-    <hyperlink r:id="rId12" ref="C13"/>
-    <hyperlink r:id="rId13" ref="C14"/>
-    <hyperlink r:id="rId14" ref="C15"/>
-    <hyperlink r:id="rId15" ref="C16"/>
-    <hyperlink r:id="rId16" ref="C18"/>
-    <hyperlink r:id="rId17" ref="C19"/>
-    <hyperlink r:id="rId18" ref="C20"/>
-    <hyperlink r:id="rId19" ref="C21"/>
-    <hyperlink r:id="rId20" ref="C22"/>
-    <hyperlink r:id="rId21" ref="C23"/>
-    <hyperlink r:id="rId22" ref="C24"/>
-    <hyperlink r:id="rId23" ref="C25"/>
-    <hyperlink r:id="rId24" ref="C26"/>
-    <hyperlink r:id="rId25" ref="C27"/>
-    <hyperlink r:id="rId26" ref="C28"/>
-    <hyperlink r:id="rId27" ref="C29"/>
-    <hyperlink r:id="rId28" ref="C30"/>
-    <hyperlink r:id="rId29" ref="C31"/>
-    <hyperlink r:id="rId30" ref="C32"/>
-    <hyperlink r:id="rId31" ref="C33"/>
-    <hyperlink r:id="rId32" ref="C34"/>
-    <hyperlink r:id="rId33" ref="C35"/>
-    <hyperlink r:id="rId34" ref="C36"/>
-    <hyperlink r:id="rId35" ref="C37"/>
-    <hyperlink r:id="rId36" ref="C38"/>
-    <hyperlink r:id="rId37" ref="C39"/>
-    <hyperlink r:id="rId38" ref="C40"/>
-    <hyperlink r:id="rId39" ref="C41"/>
-    <hyperlink r:id="rId40" ref="C42"/>
-    <hyperlink r:id="rId41" ref="C43"/>
-    <hyperlink r:id="rId42" ref="C44"/>
-    <hyperlink r:id="rId43" ref="C45"/>
+    <hyperlink r:id="rId1" ref="D2"/>
+    <hyperlink r:id="rId2" ref="D3"/>
+    <hyperlink r:id="rId3" ref="D4"/>
+    <hyperlink r:id="rId4" ref="D5"/>
+    <hyperlink r:id="rId5" ref="D6"/>
+    <hyperlink r:id="rId6" ref="D7"/>
+    <hyperlink r:id="rId7" ref="D8"/>
+    <hyperlink r:id="rId8" ref="D9"/>
+    <hyperlink r:id="rId9" ref="D10"/>
+    <hyperlink r:id="rId10" ref="D11"/>
+    <hyperlink r:id="rId11" ref="D12"/>
+    <hyperlink r:id="rId12" ref="D13"/>
+    <hyperlink r:id="rId13" ref="D14"/>
+    <hyperlink r:id="rId14" ref="D15"/>
+    <hyperlink r:id="rId15" ref="D16"/>
+    <hyperlink r:id="rId16" ref="D17"/>
+    <hyperlink r:id="rId17" ref="D18"/>
+    <hyperlink r:id="rId18" ref="D19"/>
+    <hyperlink r:id="rId19" ref="D20"/>
+    <hyperlink r:id="rId20" ref="D21"/>
+    <hyperlink r:id="rId21" ref="D22"/>
+    <hyperlink r:id="rId22" ref="D23"/>
+    <hyperlink r:id="rId23" ref="D24"/>
+    <hyperlink r:id="rId24" ref="D25"/>
+    <hyperlink r:id="rId25" ref="D26"/>
+    <hyperlink r:id="rId26" ref="D27"/>
+    <hyperlink r:id="rId27" ref="D28"/>
+    <hyperlink r:id="rId28" ref="D29"/>
+    <hyperlink r:id="rId29" ref="D30"/>
+    <hyperlink r:id="rId30" ref="D31"/>
+    <hyperlink r:id="rId31" ref="D32"/>
+    <hyperlink r:id="rId32" ref="D33"/>
+    <hyperlink r:id="rId33" ref="D34"/>
+    <hyperlink r:id="rId34" ref="D35"/>
+    <hyperlink r:id="rId35" ref="D36"/>
+    <hyperlink r:id="rId36" ref="D37"/>
+    <hyperlink r:id="rId37" ref="D38"/>
+    <hyperlink r:id="rId38" ref="D39"/>
+    <hyperlink r:id="rId39" ref="D40"/>
+    <hyperlink r:id="rId40" ref="D41"/>
+    <hyperlink r:id="rId41" ref="D42"/>
+    <hyperlink r:id="rId42" ref="D43"/>
+    <hyperlink r:id="rId43" ref="D44"/>
+    <hyperlink r:id="rId44" ref="D45"/>
+    <hyperlink r:id="rId45" ref="D47"/>
   </hyperlinks>
-  <drawing r:id="rId44"/>
+  <drawing r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>